<commit_message>
Day 21 - steps
</commit_message>
<xml_diff>
--- a/AoC2018_21_steps.xlsx
+++ b/AoC2018_21_steps.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="99">
   <si>
     <t>addi 5 1 5</t>
   </si>
@@ -315,6 +315,12 @@
   </si>
   <si>
     <t>Beeinflussung von Reg 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> …</t>
   </si>
 </sst>
 </file>
@@ -698,11 +704,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O95"/>
+  <dimension ref="A1:O97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K28" sqref="K28"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A96" sqref="A96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -3628,6 +3634,16 @@
         <v>88</v>
       </c>
     </row>
+    <row r="96" spans="1:12">
+      <c r="A96" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="97" spans="6:6">
+      <c r="F97" t="s">
+        <v>97</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>